<commit_message>
not proper closed commit, still working on broch
Looking into MALN, needed to correct for area of plant vs segment, just like was done for MALC
production looks good, cannot get carbon content to respond properly, also not enough frond area growth, and nitrogen storage increases too fast. I think that maybe the seasonal growth needs to be adjusted so it actually = 2 at max
</commit_message>
<xml_diff>
--- a/documentation/unit_conversions_from_paper_per_area.xlsx
+++ b/documentation/unit_conversions_from_paper_per_area.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\MALG\documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18690" windowHeight="12585" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18690" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="State variables" sheetId="7" r:id="rId1"/>
@@ -19,12 +14,12 @@
     <sheet name="MALDIS" sheetId="6" r:id="rId5"/>
     <sheet name="equations exploration" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="140">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -155,9 +150,6 @@
     <t>gN/m3</t>
   </si>
   <si>
-    <t>kn</t>
-  </si>
-  <si>
     <t>N:C ratio in structural mass</t>
   </si>
   <si>
@@ -429,12 +421,33 @@
   </si>
   <si>
     <t>Reference respiration rate at T2</t>
+  </si>
+  <si>
+    <t>value in Broch</t>
+  </si>
+  <si>
+    <t>conversion</t>
+  </si>
+  <si>
+    <t>umol/l</t>
+  </si>
+  <si>
+    <t>gN/dm2/hr</t>
+  </si>
+  <si>
+    <t>gN/gC</t>
+  </si>
+  <si>
+    <t>NCRatMALS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -522,6 +535,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,11 +851,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="244072328"/>
-        <c:axId val="244075072"/>
+        <c:axId val="78838784"/>
+        <c:axId val="79192832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="244072328"/>
+        <c:axId val="78838784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,12 +865,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244075072"/>
+        <c:crossAx val="79192832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="244075072"/>
+        <c:axId val="79192832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,7 +881,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244072328"/>
+        <c:crossAx val="78838784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -965,7 +980,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1000,7 +1015,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1255,37 +1270,37 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
         <v>123</v>
-      </c>
-      <c r="C6" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7">
         <v>0.2</v>
       </c>
       <c r="C7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1363,7 +1378,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D4" s="6">
         <v>-999</v>
@@ -1408,7 +1423,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1466,10 +1481,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>36</v>
@@ -1482,13 +1497,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="D12" s="6">
         <v>-999</v>
@@ -1598,10 +1613,10 @@
         <v>28</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D19" s="7">
         <f>0.22 / 0.01</f>
@@ -1612,7 +1627,7 @@
     </row>
     <row r="20" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1625,25 +1640,25 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1676,10 +1691,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,10 +1703,11 @@
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1704,10 +1720,17 @@
       <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
@@ -1715,11 +1738,10 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="16"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>39</v>
       </c>
@@ -1733,11 +1755,10 @@
         <v>-999</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="16"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1751,12 +1772,10 @@
         <v>-999</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="6">
-        <f>6*0.6</f>
-        <v>3.5999999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="16"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>40</v>
       </c>
@@ -1770,9 +1789,10 @@
         <v>-999</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="16"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -1786,19 +1806,21 @@
         <v>-999</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="16"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="16"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
@@ -1812,158 +1834,175 @@
         <v>0.01</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="16"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="6">
-        <v>0.01</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="16"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="D10" s="6">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="16"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="6">
-        <f>4*F11*0.001</f>
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <f>E11*G11</f>
+        <v>1.264516129032258E-2</v>
+      </c>
+      <c r="E11" s="6">
+        <v>4</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="6">
+        <f>(14/(14+(16*3)))*14/1000</f>
+        <v>3.1612903225806451E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="6">
+        <f>D11</f>
+        <v>1.264516129032258E-2</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="19">
+        <f>E13*G13</f>
+        <v>0.33599999999999997</v>
+      </c>
+      <c r="E13" s="18">
+        <v>1.3999999999999999E-4</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G13" s="6">
+        <f>100*24</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="6">
-        <f>4*F12*0.001</f>
-        <v>0.12388</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6">
-        <v>30.97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="C14" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="D13" s="6">
-        <f>0.00014*24*100</f>
+      <c r="D14" s="19">
+        <f>D13</f>
         <v>0.33599999999999997</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6">
-        <f>D13*F12/F11</f>
-        <v>0.74327999999999983</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="D14" s="16">
-        <f>D13*F12/F11</f>
-        <v>0.74327999999999983</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="D15" s="6">
         <v>-999</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="16"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="7">
         <v>0.03</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="16"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="16"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>8</v>
       </c>
@@ -1971,15 +2010,17 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="16"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1990,7 +2031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -2066,7 +2107,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2092,13 +2133,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>73</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="6">
         <v>-999</v>
@@ -2111,10 +2152,10 @@
         <v>15</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D8" s="6">
         <f>273+15</f>
@@ -2125,13 +2166,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D9" s="6">
         <f>24 *0.00122*100</f>
@@ -2144,13 +2185,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D10" s="6">
         <f>0.00144 * 24 * 100</f>
@@ -2163,13 +2204,13 @@
     </row>
     <row r="11" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>132</v>
-      </c>
       <c r="C11" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D11" s="15">
         <f>0.0002785 * 100 *24</f>
@@ -2180,13 +2221,13 @@
     </row>
     <row r="12" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>134</v>
-      </c>
       <c r="C12" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12" s="15">
         <f>0.0005429 * 100 *24</f>
@@ -2197,13 +2238,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="6">
         <f>285</f>
@@ -2214,13 +2255,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" s="6">
         <f>290</f>
@@ -2231,13 +2272,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15">
         <f>1694.4-273</f>
@@ -2246,13 +2287,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D16" s="6">
         <f>25924</f>
@@ -2263,13 +2304,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" s="6">
         <v>27774</v>
@@ -2279,13 +2320,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="D18" s="6">
         <v>11033</v>
@@ -2295,13 +2336,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" s="6">
         <v>-999</v>
@@ -2311,13 +2352,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" s="6">
         <v>-999</v>
@@ -2327,13 +2368,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="D21" s="6">
         <f>0.0000375*100*24</f>
@@ -2344,13 +2385,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="C22" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="7">
         <f>200</f>
@@ -2361,7 +2402,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -2397,7 +2438,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2405,7 +2446,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28">
         <v>-1</v>
@@ -2525,7 +2566,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -2533,13 +2574,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
@@ -2547,13 +2588,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="D9" s="6">
         <v>0.1</v>
@@ -2561,13 +2602,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
@@ -2575,13 +2616,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="C11" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" s="6">
         <v>-999</v>
@@ -2595,7 +2636,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -2608,7 +2649,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -2622,7 +2663,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2656,16 +2697,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1">
         <v>0.1085</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2685,7 +2726,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3">
         <v>6</v>

</xml_diff>